<commit_message>
With images and coding list of weather conditions
</commit_message>
<xml_diff>
--- a/Weather App.xlsx
+++ b/Weather App.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorbita\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\My Personal Projects\Weather App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{046F60BA-A5D6-4E9C-8ED1-7ED492EA91D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACF4160-0BF7-4FF0-AB0A-F427F6D79761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="570" windowWidth="24240" windowHeight="13020" xr2:uid="{EDA625D9-2D5F-4BC7-8038-864FE80252AF}"/>
+    <workbookView xWindow="-24120" yWindow="570" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{EDA625D9-2D5F-4BC7-8038-864FE80252AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="images &amp; icon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Today</t>
   </si>
@@ -70,13 +71,244 @@
   </si>
   <si>
     <t>atmospheric ground level(hPa)</t>
+  </si>
+  <si>
+    <t>Group 2xx: Thunderstorm</t>
+  </si>
+  <si>
+    <t>Thunderstorm</t>
+  </si>
+  <si>
+    <t>thunderstorm with light rain</t>
+  </si>
+  <si>
+    <t>thunderstorm with rain</t>
+  </si>
+  <si>
+    <t>thunderstorm with heavy rain</t>
+  </si>
+  <si>
+    <t>light thunderstorm</t>
+  </si>
+  <si>
+    <t>thunderstorm</t>
+  </si>
+  <si>
+    <t>heavy thunderstorm</t>
+  </si>
+  <si>
+    <t>ragged thunderstorm</t>
+  </si>
+  <si>
+    <t>thunderstorm with light drizzle</t>
+  </si>
+  <si>
+    <t>thunderstorm with drizzle</t>
+  </si>
+  <si>
+    <t>thunderstorm with heavy drizzle</t>
+  </si>
+  <si>
+    <t>Group 3xx: Drizzle</t>
+  </si>
+  <si>
+    <t>Drizzle</t>
+  </si>
+  <si>
+    <t>light intensity drizzle</t>
+  </si>
+  <si>
+    <t>drizzle</t>
+  </si>
+  <si>
+    <t>heavy intensity drizzle</t>
+  </si>
+  <si>
+    <t>light intensity drizzle rain</t>
+  </si>
+  <si>
+    <t>drizzle rain</t>
+  </si>
+  <si>
+    <t>heavy intensity drizzle rain</t>
+  </si>
+  <si>
+    <t>shower rain and drizzle</t>
+  </si>
+  <si>
+    <t>heavy shower rain and drizzle</t>
+  </si>
+  <si>
+    <t>shower drizzle</t>
+  </si>
+  <si>
+    <t>Group 5xx: Rain</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>light rain</t>
+  </si>
+  <si>
+    <t>moderate rain</t>
+  </si>
+  <si>
+    <t>heavy intensity rain</t>
+  </si>
+  <si>
+    <t>very heavy rain</t>
+  </si>
+  <si>
+    <t>extreme rain</t>
+  </si>
+  <si>
+    <t>freezing rain</t>
+  </si>
+  <si>
+    <t>light intensity shower rain</t>
+  </si>
+  <si>
+    <t>shower rain</t>
+  </si>
+  <si>
+    <t>heavy intensity shower rain</t>
+  </si>
+  <si>
+    <t>ragged shower rain</t>
+  </si>
+  <si>
+    <t>Group 6xx: Snow</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>light snow</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>heavy snow</t>
+  </si>
+  <si>
+    <t>sleet</t>
+  </si>
+  <si>
+    <t>light shower sleet</t>
+  </si>
+  <si>
+    <t>shower sleet</t>
+  </si>
+  <si>
+    <t>light rain and snow</t>
+  </si>
+  <si>
+    <t>rain and snow</t>
+  </si>
+  <si>
+    <t>light shower snow</t>
+  </si>
+  <si>
+    <t>shower snow</t>
+  </si>
+  <si>
+    <t>heavy shower snow</t>
+  </si>
+  <si>
+    <t>Group 7xx: Atmosphere</t>
+  </si>
+  <si>
+    <t>Mist</t>
+  </si>
+  <si>
+    <t>mist</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>smoke</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>haze</t>
+  </si>
+  <si>
+    <t>Dust</t>
+  </si>
+  <si>
+    <t>sand/dust whirls</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>fog</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>dust</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>volcanic ash</t>
+  </si>
+  <si>
+    <t>Squall</t>
+  </si>
+  <si>
+    <t>squalls</t>
+  </si>
+  <si>
+    <t>Tornado</t>
+  </si>
+  <si>
+    <t>tornado</t>
+  </si>
+  <si>
+    <t>Group 800: Clear</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>clear sky</t>
+  </si>
+  <si>
+    <t>Group 80x: Clouds</t>
+  </si>
+  <si>
+    <t>Clouds</t>
+  </si>
+  <si>
+    <t>few clouds: 11-25%</t>
+  </si>
+  <si>
+    <t>scattered clouds: 25-50%</t>
+  </si>
+  <si>
+    <t>broken clouds: 51-84%</t>
+  </si>
+  <si>
+    <t>overcast clouds: 85-100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +316,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF48484A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,12 +345,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC105BC8-EEDB-4D16-8EC8-A4B06C7AF02E}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,4 +808,664 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2A9A10-A3D3-4AAA-87C1-6BC4E5834DC5}">
+  <dimension ref="A2:C63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>200</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>201</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>202</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>210</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>211</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>212</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>221</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>230</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>231</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>232</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>300</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>301</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>302</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>310</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>311</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>312</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>313</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>314</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>321</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>500</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>501</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>502</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>503</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>504</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>511</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>520</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>521</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>522</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>531</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>600</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>601</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>602</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>611</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>612</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>613</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>615</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>616</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>620</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>621</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>622</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>701</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>711</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>721</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>731</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>741</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>751</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>761</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>762</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>771</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>781</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>800</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>801</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>802</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>803</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>804</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Almost doen with Today Forecast
</commit_message>
<xml_diff>
--- a/Weather App.xlsx
+++ b/Weather App.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\My Personal Projects\Weather App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\My Personal Projects\weather-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACF4160-0BF7-4FF0-AB0A-F427F6D79761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="570" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{EDA625D9-2D5F-4BC7-8038-864FE80252AF}"/>
+    <workbookView xWindow="-24120" yWindow="570" windowWidth="24240" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="images &amp; icon" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
   <si>
     <t>Today</t>
   </si>
@@ -302,12 +301,36 @@
   </si>
   <si>
     <t>overcast clouds: 85-100%</t>
+  </si>
+  <si>
+    <t>thunderstorm.png</t>
+  </si>
+  <si>
+    <t>drizzle.png</t>
+  </si>
+  <si>
+    <t>rain.png</t>
+  </si>
+  <si>
+    <t>freezing-rain.png</t>
+  </si>
+  <si>
+    <t>snow.png</t>
+  </si>
+  <si>
+    <t>fog.png</t>
+  </si>
+  <si>
+    <t>sun.png</t>
+  </si>
+  <si>
+    <t>clouds.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,25 +709,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC105BC8-EEDB-4D16-8EC8-A4B06C7AF02E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -712,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -720,7 +743,7 @@
         <v>306.20999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -728,7 +751,7 @@
         <v>313.20999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -736,7 +759,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -744,7 +767,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -752,12 +775,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -765,7 +788,7 @@
         <v>1730150669</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -773,7 +796,7 @@
         <v>1730193437</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -781,7 +804,7 @@
         <v>306.20999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -789,7 +812,7 @@
         <v>306.20999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -797,7 +820,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -811,26 +834,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2A9A10-A3D3-4AAA-87C1-6BC4E5834DC5}">
-  <dimension ref="A2:C63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -840,8 +864,11 @@
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>201</v>
       </c>
@@ -851,8 +878,11 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>202</v>
       </c>
@@ -862,8 +892,11 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>210</v>
       </c>
@@ -873,8 +906,11 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>211</v>
       </c>
@@ -884,8 +920,11 @@
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>212</v>
       </c>
@@ -895,8 +934,11 @@
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>221</v>
       </c>
@@ -906,8 +948,11 @@
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>230</v>
       </c>
@@ -917,8 +962,11 @@
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>231</v>
       </c>
@@ -928,8 +976,11 @@
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>232</v>
       </c>
@@ -939,13 +990,16 @@
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>300</v>
       </c>
@@ -955,8 +1009,11 @@
       <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>301</v>
       </c>
@@ -966,8 +1023,11 @@
       <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>302</v>
       </c>
@@ -977,8 +1037,11 @@
       <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>310</v>
       </c>
@@ -988,8 +1051,11 @@
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>311</v>
       </c>
@@ -999,8 +1065,11 @@
       <c r="C18" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>312</v>
       </c>
@@ -1010,8 +1079,11 @@
       <c r="C19" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>313</v>
       </c>
@@ -1021,8 +1093,11 @@
       <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>314</v>
       </c>
@@ -1032,8 +1107,11 @@
       <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>321</v>
       </c>
@@ -1043,13 +1121,16 @@
       <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>500</v>
       </c>
@@ -1059,8 +1140,11 @@
       <c r="C24" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>501</v>
       </c>
@@ -1070,8 +1154,11 @@
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>502</v>
       </c>
@@ -1081,8 +1168,11 @@
       <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>503</v>
       </c>
@@ -1092,8 +1182,11 @@
       <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>504</v>
       </c>
@@ -1103,8 +1196,11 @@
       <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>511</v>
       </c>
@@ -1114,8 +1210,11 @@
       <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>520</v>
       </c>
@@ -1125,8 +1224,11 @@
       <c r="C30" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>521</v>
       </c>
@@ -1136,8 +1238,11 @@
       <c r="C31" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>522</v>
       </c>
@@ -1147,8 +1252,11 @@
       <c r="C32" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>531</v>
       </c>
@@ -1158,13 +1266,16 @@
       <c r="C33" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>600</v>
       </c>
@@ -1174,8 +1285,11 @@
       <c r="C35" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>601</v>
       </c>
@@ -1185,8 +1299,11 @@
       <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>602</v>
       </c>
@@ -1196,8 +1313,11 @@
       <c r="C37" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>611</v>
       </c>
@@ -1207,8 +1327,11 @@
       <c r="C38" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>612</v>
       </c>
@@ -1218,8 +1341,11 @@
       <c r="C39" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>613</v>
       </c>
@@ -1229,8 +1355,11 @@
       <c r="C40" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>615</v>
       </c>
@@ -1240,8 +1369,11 @@
       <c r="C41" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>616</v>
       </c>
@@ -1251,8 +1383,11 @@
       <c r="C42" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>620</v>
       </c>
@@ -1262,8 +1397,11 @@
       <c r="C43" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>621</v>
       </c>
@@ -1273,8 +1411,11 @@
       <c r="C44" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>622</v>
       </c>
@@ -1284,13 +1425,16 @@
       <c r="C45" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>701</v>
       </c>
@@ -1300,8 +1444,11 @@
       <c r="C47" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>711</v>
       </c>
@@ -1311,8 +1458,11 @@
       <c r="C48" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>721</v>
       </c>
@@ -1322,8 +1472,11 @@
       <c r="C49" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>731</v>
       </c>
@@ -1333,8 +1486,11 @@
       <c r="C50" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>741</v>
       </c>
@@ -1344,8 +1500,11 @@
       <c r="C51" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>751</v>
       </c>
@@ -1355,8 +1514,11 @@
       <c r="C52" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>761</v>
       </c>
@@ -1366,8 +1528,11 @@
       <c r="C53" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>762</v>
       </c>
@@ -1377,8 +1542,11 @@
       <c r="C54" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>771</v>
       </c>
@@ -1388,8 +1556,11 @@
       <c r="C55" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>781</v>
       </c>
@@ -1399,13 +1570,16 @@
       <c r="C56" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E56" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>800</v>
       </c>
@@ -1415,13 +1589,16 @@
       <c r="C58" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>801</v>
       </c>
@@ -1431,8 +1608,11 @@
       <c r="C60" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>802</v>
       </c>
@@ -1442,8 +1622,11 @@
       <c r="C61" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>803</v>
       </c>
@@ -1453,8 +1636,11 @@
       <c r="C62" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>804</v>
       </c>
@@ -1463,6 +1649,9 @@
       </c>
       <c r="C63" s="3" t="s">
         <v>91</v>
+      </c>
+      <c r="E63" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>